<commit_message>
[Ankur] Hotel code update
</commit_message>
<xml_diff>
--- a/data/excel/SBT_Hotel.xlsx
+++ b/data/excel/SBT_Hotel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33A63D4-D10E-4B11-9E8E-4BE578A69A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E9670D-AC47-4755-94BD-CCF2399410CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="327">
   <si>
     <t>Fop</t>
   </si>
@@ -1012,6 +1012,21 @@
   </si>
   <si>
     <t>21-Dec-2023</t>
+  </si>
+  <si>
+    <t>LoginType</t>
+  </si>
+  <si>
+    <t>Emailid</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>test.quadlabs.net</t>
+  </si>
+  <si>
+    <t>Old Url</t>
   </si>
 </sst>
 </file>
@@ -1798,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2663B78-477A-4A80-9FFF-53D3FC78CF07}">
-  <dimension ref="A1:CA2"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
-      <selection activeCell="BZ6" sqref="BZ6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,83 +1825,86 @@
     <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="18" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="19" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="18" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>120</v>
       </c>
@@ -1900,232 +1918,241 @@
         <v>37</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="K1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="M1" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="N1" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="O1" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="AB1" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="AC1" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="AB1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>314</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AO1" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AP1" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="AN1" s="33" t="s">
+      <c r="AQ1" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="AO1" s="33" t="s">
+      <c r="AR1" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="AP1" s="33" t="s">
+      <c r="AS1" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="AQ1" s="23" t="s">
+      <c r="AT1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="AR1" s="33" t="s">
+      <c r="AU1" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="AS1" s="33" t="s">
+      <c r="AV1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="AT1" s="23" t="s">
+      <c r="AW1" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="AU1" s="23" t="s">
+      <c r="AX1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="AV1" s="23" t="s">
+      <c r="AY1" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="AW1" s="23" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="AX1" s="23" t="s">
+      <c r="BA1" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="AY1" s="23" t="s">
+      <c r="BB1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="AZ1" s="23" t="s">
+      <c r="BC1" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="BA1" s="23" t="s">
+      <c r="BD1" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="BB1" s="23" t="s">
+      <c r="BE1" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="BC1" s="23" t="s">
+      <c r="BF1" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="BD1" s="23" t="s">
+      <c r="BG1" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="BE1" s="23" t="s">
+      <c r="BH1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="BF1" s="23" t="s">
+      <c r="BI1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="BG1" s="23" t="s">
+      <c r="BJ1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="BH1" s="23" t="s">
+      <c r="BK1" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="BI1" s="23" t="s">
+      <c r="BL1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="BJ1" s="23" t="s">
+      <c r="BM1" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="BK1" s="23" t="s">
+      <c r="BN1" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="BL1" s="23" t="s">
+      <c r="BO1" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="BM1" s="23" t="s">
+      <c r="BP1" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="BN1" s="23" t="s">
+      <c r="BQ1" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="BO1" s="23" t="s">
+      <c r="BR1" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="BP1" s="23" t="s">
+      <c r="BS1" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="BQ1" s="23" t="s">
+      <c r="BT1" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="BR1" s="23" t="s">
+      <c r="BU1" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="BS1" s="23" t="s">
+      <c r="BV1" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="BT1" s="23" t="s">
+      <c r="BW1" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="BU1" s="23" t="s">
+      <c r="BX1" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="BV1" s="23" t="s">
+      <c r="BY1" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="BW1" s="23" t="s">
+      <c r="BZ1" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="BX1" s="23" t="s">
+      <c r="CA1" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="BY1" s="23" t="s">
+      <c r="CB1" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="BZ1" s="23" t="s">
+      <c r="CC1" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="CA1" s="23" t="s">
+      <c r="CD1" s="23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>147</v>
       </c>
@@ -2139,322 +2166,337 @@
         <v>164</v>
       </c>
       <c r="E2" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="I2" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="K2" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="O2" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="R2" s="32" t="s">
+      <c r="U2" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="V2" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="T2" s="24">
+      <c r="W2" s="24">
         <v>2</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="Z2" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="AA2" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="Y2" s="24">
+      <c r="AB2" s="24">
         <v>3</v>
       </c>
-      <c r="Z2" s="24">
+      <c r="AC2" s="24">
         <v>3</v>
       </c>
-      <c r="AA2" s="24">
+      <c r="AD2" s="24">
         <v>3</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AE2" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AF2" s="24" t="s">
         <v>40</v>
-      </c>
-      <c r="AD2" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE2" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF2" s="24" t="s">
-        <v>232</v>
       </c>
       <c r="AG2" s="24" t="s">
         <v>229</v>
       </c>
       <c r="AH2" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI2" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK2" s="24" t="s">
         <v>309</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="AJ2" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="AK2" s="26" t="s">
-        <v>234</v>
       </c>
       <c r="AL2" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="AM2" s="24">
+      <c r="AM2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP2" s="24">
         <v>2</v>
       </c>
-      <c r="AN2" s="24" t="s">
+      <c r="AQ2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AO2" s="37" t="s">
+      <c r="AR2" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="AP2" s="37" t="s">
+      <c r="AS2" s="37" t="s">
         <v>235</v>
-      </c>
-      <c r="AQ2" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="AR2" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS2" s="37" t="s">
-        <v>236</v>
       </c>
       <c r="AT2" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="AU2" s="24" t="s">
+      <c r="AU2" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="AW2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX2" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AY2" t="s">
         <v>238</v>
       </c>
-      <c r="AW2" s="24" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="AX2" s="24" t="s">
+      <c r="BA2" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AZ2" s="41" t="s">
+      <c r="BC2" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="BB2" s="41" t="s">
+      <c r="BE2" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="BC2" s="42" t="s">
+      <c r="BF2" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="BD2" s="42" t="s">
+      <c r="BG2" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="BE2" s="24">
+      <c r="BH2" s="24">
         <v>2</v>
       </c>
-      <c r="BF2" s="24">
+      <c r="BI2" s="24">
         <v>1</v>
       </c>
-      <c r="BG2" s="24">
+      <c r="BJ2" s="24">
         <v>1</v>
       </c>
-      <c r="BH2" s="24" t="s">
+      <c r="BK2" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="BI2" s="24" t="s">
+      <c r="BL2" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="BJ2" s="24" t="s">
+      <c r="BM2" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="BK2" s="26" t="s">
+      <c r="BN2" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="BL2" s="24" t="s">
+      <c r="BO2" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="BM2" s="24" t="s">
+      <c r="BP2" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="BN2" s="24">
+      <c r="BQ2" s="24">
         <v>25</v>
       </c>
-      <c r="BO2" s="24" t="s">
+      <c r="BR2" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="BP2" s="24" t="s">
+      <c r="BS2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="BQ2" s="24" t="s">
+      <c r="BT2" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="BR2" s="26" t="s">
+      <c r="BU2" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="BS2" s="24" t="s">
+      <c r="BV2" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="BT2" s="24" t="s">
+      <c r="BW2" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="BU2" s="24" t="s">
+      <c r="BX2" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="BV2" s="24" t="s">
+      <c r="BY2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="BW2" s="43" t="s">
+      <c r="BZ2" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="BX2" s="26" t="s">
+      <c r="CA2" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="BY2" s="43" t="s">
+      <c r="CB2" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="BZ2" s="26" t="s">
+      <c r="CC2" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="CA2" s="39" t="s">
+      <c r="CD2" s="39" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="28">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2 AH2" xr:uid="{1A3610A5-ECFA-492A-A489-37C96F899B80}">
+  <dataValidations count="30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2 AK2" xr:uid="{1A3610A5-ECFA-492A-A489-37C96F899B80}">
       <formula1>"5 KM,10 KM,20 KM,30 KM,40 KM,50 KM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{9C19A42A-D89D-4DDE-A4C8-1F1B2743585E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{9C19A42A-D89D-4DDE-A4C8-1F1B2743585E}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CA2" xr:uid="{A8B41F32-A2C0-478A-86BA-8E141CEEE5B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CD2" xr:uid="{A8B41F32-A2C0-478A-86BA-8E141CEEE5B5}">
       <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{AAF114E8-A236-4AE5-806A-C78913C137C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{AAF114E8-A236-4AE5-806A-C78913C137C3}">
       <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{7779DB6C-5818-4915-9A07-02B7C4F6B2AF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{7779DB6C-5818-4915-9A07-02B7C4F6B2AF}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{37CB28C1-8D14-42C1-9757-952A8A4818B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{37CB28C1-8D14-42C1-9757-952A8A4818B3}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{80C00CFD-CD64-4121-A897-C010A502ED4A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{80C00CFD-CD64-4121-A897-C010A502ED4A}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{091C247D-06C5-4FD7-8F70-2C1E838A460E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{091C247D-06C5-4FD7-8F70-2C1E838A460E}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{8720B9F1-353B-4087-B0CF-D6DD3898ED4E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{8720B9F1-353B-4087-B0CF-D6DD3898ED4E}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE2:BG2" xr:uid="{1FAAD004-7F32-49EA-B311-C8D1210FD73B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BJ2" xr:uid="{1FAAD004-7F32-49EA-B311-C8D1210FD73B}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{2F394A1B-1399-42F6-8A1F-A6107D2AD137}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{2F394A1B-1399-42F6-8A1F-A6107D2AD137}">
       <formula1>"Economy,Premium Economy,Business Class,First Class"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{54EF34A0-0AB1-491D-9588-1CE451363497}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{54EF34A0-0AB1-491D-9588-1CE451363497}">
       <formula1>"Hotel,Apartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{1C77E60E-3F8A-44D2-A112-FCE8C42518AD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2" xr:uid="{1C77E60E-3F8A-44D2-A112-FCE8C42518AD}">
       <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{3A159A86-6693-4F7B-A136-06CFEA738A20}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{3A159A86-6693-4F7B-A136-06CFEA738A20}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2" xr:uid="{FEF861A3-51ED-43C0-B28A-BE3EB50513E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2" xr:uid="{FEF861A3-51ED-43C0-B28A-BE3EB50513E4}">
       <formula1>"Hotel,Hotel+Flight,Hotel+Car,Hotel+Flight+Car,Hotel+Car+Flight"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2" xr:uid="{2128310B-E046-4186-898C-B1B47CA85B1F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2" xr:uid="{2128310B-E046-4186-898C-B1B47CA85B1F}">
       <formula1>"MasterCard,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2" xr:uid="{524E775D-F779-431E-B57A-0D09D5C33E50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CA2" xr:uid="{524E775D-F779-431E-B57A-0D09D5C33E50}">
       <formula1>"5123456789012346,4111111111111111"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2" xr:uid="{C3D9C8E7-F169-45B4-9589-7816A1C423AC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2" xr:uid="{C3D9C8E7-F169-45B4-9589-7816A1C423AC}">
       <formula1>"Quote,BookAndQuote,Fulfilment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2 AT2 AQ2:AR2 AD2 AI2 AB2 AG2 BO2 AL2" xr:uid="{626BF180-88BC-473D-86A0-BED78CBB0A22}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2 AW2 AT2:AU2 AG2 AL2 AE2 AJ2 BR2 AO2" xr:uid="{626BF180-88BC-473D-86A0-BED78CBB0A22}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 AC2" xr:uid="{B6A172F9-1570-47CE-8EBD-679A7B8A20BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2 AF2" xr:uid="{B6A172F9-1570-47CE-8EBD-679A7B8A20BC}">
       <formula1>"Individual,Dependent,Personal,Guest"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{AF1F245C-F5C8-4D1D-B5C8-900E635A7B65}">
       <formula1>"sbt,preprod117,Live"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{9AE0CBBB-F3CD-4653-BF77-58ED53B5C627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2" xr:uid="{9AE0CBBB-F3CD-4653-BF77-58ED53B5C627}">
       <formula1>"OneWay,RoundTrip,MultiCity"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BV2" xr:uid="{5A701C4E-D11A-4206-843D-A5EE38C499FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2" xr:uid="{5A701C4E-D11A-4206-843D-A5EE38C499FD}">
       <formula1>"Credit Card,Bill To Company"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{4CE3F444-FD09-47FC-B12F-AFEB6FD7C7F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{4CE3F444-FD09-47FC-B12F-AFEB6FD7C7F6}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2" xr:uid="{49EE4478-AAE1-4831-B450-9BB5A6CF33F3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2" xr:uid="{49EE4478-AAE1-4831-B450-9BB5A6CF33F3}">
       <formula1>"SendForApproval,ProceedToCheckout"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{E7F00521-023F-4D90-9127-367B050517F5}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{7AF69C06-712F-47A3-8CF4-3AA749857B70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{7AF69C06-712F-47A3-8CF4-3AA749857B70}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{4EA60C40-CBED-4436-81AD-7AEDED4DD7CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{4EA60C40-CBED-4436-81AD-7AEDED4DD7CE}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{212CEDE3-32A2-490D-B074-8F6814274A7B}">
+      <formula1>"Old Url,SSO Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{24EFDCBF-B153-41D7-BACD-CEB6FF3B832C}">
+      <formula1>"sachin.kumar@quadlabs.com"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="Admin@123" xr:uid="{F8B10C09-66E6-42AC-8295-AEF5443AE37C}"/>
-    <hyperlink ref="L2" r:id="rId2" display="prince.chaurasia@quadlabs.com" xr:uid="{82DEF3E1-6F1D-457E-BE1F-5A6E173461AB}"/>
+    <hyperlink ref="K2" r:id="rId1" display="Admin@123" xr:uid="{F8B10C09-66E6-42AC-8295-AEF5443AE37C}"/>
+    <hyperlink ref="O2" r:id="rId2" display="prince.chaurasia@quadlabs.com" xr:uid="{82DEF3E1-6F1D-457E-BE1F-5A6E173461AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Ankur] Add Other services
</commit_message>
<xml_diff>
--- a/data/excel/SBT_Hotel.xlsx
+++ b/data/excel/SBT_Hotel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B4E14-6643-4485-B454-3E377F10108E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB5B499-AE1F-476E-93C7-8F2777EF8F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Business" sheetId="13" r:id="rId1"/>
@@ -24,19 +24,21 @@
     <sheet name="Sheet11" sheetId="27" r:id="rId9"/>
     <sheet name="Sheet13" sheetId="29" r:id="rId10"/>
     <sheet name="Sheet14" sheetId="30" r:id="rId11"/>
-    <sheet name="Sheet15" sheetId="31" r:id="rId12"/>
-    <sheet name="Sheet12" sheetId="28" r:id="rId13"/>
-    <sheet name="Sheet3" sheetId="18" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="17" r:id="rId15"/>
-    <sheet name="Sheet4" sheetId="19" r:id="rId16"/>
-    <sheet name="Dependent" sheetId="5" r:id="rId17"/>
-    <sheet name="Sheet1" sheetId="16" r:id="rId18"/>
-    <sheet name="Personal" sheetId="6" r:id="rId19"/>
-    <sheet name="Guest" sheetId="11" r:id="rId20"/>
-    <sheet name="GuestSheet1" sheetId="15" r:id="rId21"/>
-    <sheet name="SearchWithHotelName" sheetId="2" r:id="rId22"/>
-    <sheet name="BookHotelWithPolicyType" sheetId="3" r:id="rId23"/>
-    <sheet name="AddToCart" sheetId="9" r:id="rId24"/>
+    <sheet name="Sheet16" sheetId="32" r:id="rId12"/>
+    <sheet name="Liveset" sheetId="33" r:id="rId13"/>
+    <sheet name="Sheet15" sheetId="31" r:id="rId14"/>
+    <sheet name="Sheet12" sheetId="28" r:id="rId15"/>
+    <sheet name="Sheet3" sheetId="18" r:id="rId16"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet4" sheetId="19" r:id="rId18"/>
+    <sheet name="Dependent" sheetId="5" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId20"/>
+    <sheet name="Personal" sheetId="6" r:id="rId21"/>
+    <sheet name="Guest" sheetId="11" r:id="rId22"/>
+    <sheet name="GuestSheet1" sheetId="15" r:id="rId23"/>
+    <sheet name="SearchWithHotelName" sheetId="2" r:id="rId24"/>
+    <sheet name="BookHotelWithPolicyType" sheetId="3" r:id="rId25"/>
+    <sheet name="AddToCart" sheetId="9" r:id="rId26"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3779" uniqueCount="369">
   <si>
     <t>Fop</t>
   </si>
@@ -1127,7 +1129,34 @@
     <t>20-May-2024</t>
   </si>
   <si>
-    <t>ankur.yadav@quadlabs.com</t>
+    <t>Old Url</t>
+  </si>
+  <si>
+    <t>23-May-2024</t>
+  </si>
+  <si>
+    <t>Hotel International booking flow for Individual (Admin)</t>
+  </si>
+  <si>
+    <t>Bom</t>
+  </si>
+  <si>
+    <t>Mumbai, Maharashtra, India (BOM-Chhatrapati Shivaji Intl.)</t>
+  </si>
+  <si>
+    <t>Lhr</t>
+  </si>
+  <si>
+    <t>22-May-2024</t>
+  </si>
+  <si>
+    <t>27-May-2024</t>
+  </si>
+  <si>
+    <t>24-May-2024</t>
+  </si>
+  <si>
+    <t>28-May-2024</t>
   </si>
 </sst>
 </file>
@@ -1936,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2663B78-477A-4A80-9FFF-53D3FC78CF07}">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,10 +2313,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>344</v>
+        <v>265</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>105</v>
@@ -2296,16 +2325,16 @@
         <v>323</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>161</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>162</v>
+        <v>266</v>
       </c>
       <c r="L2" s="38" t="s">
         <v>158</v>
@@ -2317,7 +2346,7 @@
         <v>269</v>
       </c>
       <c r="O2" s="30" t="s">
-        <v>359</v>
+        <v>105</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>40</v>
@@ -2627,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974A3E0D-052E-4767-B170-38FEFE199448}">
   <dimension ref="A1:CQ3"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="A1:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3718,6 +3747,2457 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E0DCA9-09F3-4C26-B3E5-E5C88853FAF5}">
+  <dimension ref="A1:CQ2"/>
+  <sheetViews>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="X1" sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="19" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="18" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD1" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF1" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG1" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="AM1" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN1" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AO1" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AP1" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="AQ1" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="AR1" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT1" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="AU1" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="AV1" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="AX1" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="AY1" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="BG1" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH1" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="BI1" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="BO1" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="BP1" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="BQ1" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="BX1" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="BY1" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="CA1" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="CB1" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="CC1" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="CD1" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="CE1" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="CF1" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="CG1" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="CH1" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="CI1" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="CJ1" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="CK1" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="CL1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="CM1" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="CN1" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="CO1" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="CP1" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="CQ1" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="R2" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA2" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD2" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE2" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF2" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG2" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="AH2" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI2" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM2" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AP2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT2" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AU2" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW2" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB2" s="24">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE2" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG2" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BH2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ2" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="BK2" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM2" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN2" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP2" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR2" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="BS2" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="BT2" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="BU2" s="24">
+        <v>2</v>
+      </c>
+      <c r="BV2" s="24">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="24">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ2" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="CA2" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="CB2" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="CC2" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="CD2" s="24">
+        <v>25</v>
+      </c>
+      <c r="CE2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG2" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH2" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="CI2" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ2" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CK2" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="CL2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM2" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="CN2" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO2" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP2" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="CQ2" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{7DADF365-01CD-4C10-ABAD-873CB2C619CF}">
+      <formula1>"LUXURY COLLECTION,COURTYARD BY MARRIOTT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{0B4EC333-7FB0-4A07-A104-2BC512CF4EE7}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{F2310514-6DF5-48A5-B81B-735B36E94D16}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{C6BAD76A-3917-484E-928E-13F4A714E497}">
+      <formula1>"//staging117/backoffice/,//preprod.quadlabs.net/backoffice/,//test.quadlabs.net/backoffice/"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{9B4F11EE-01F7-407D-AB8D-0871454CDD55}">
+      <formula1>"at,QL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{4FC18CE8-24F9-485D-A3A6-CC5F8594A47B}">
+      <formula1>"Saurav_at,tarun"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{A633F555-A6AF-4F3E-999C-F0D8BB3191F2}">
+      <formula1>"Laxmi@123,Password@123,Quad@720,Quad@721,Password@1234,Admin@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2 AW2" xr:uid="{CC6E1546-EFC3-4989-A882-C6AF9F68C4CD}">
+      <formula1>"5 KM,10 KM,20 KM,30 KM,40 KM,50 KM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{68F3548F-5CC9-47EA-A3E2-61D847BEA52C}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CQ2" xr:uid="{89710FD2-DDF2-4BCC-B365-0C7B7C0DCA4D}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar,Shekhar Singh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{F71D6F54-FB38-4725-9EBE-4CF2D383DFF0}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{8E21E9E5-942A-419D-BB44-491EF9D55C5D}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{9FA2DA59-6DAE-46AF-BEC6-0DE6F09D297A}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{2DCE42F9-8FA3-415B-9BC4-D92C292C9A7E}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{52444CAB-47D2-4E2C-88FF-CBC8E0035E9D}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2:BW2" xr:uid="{40C88515-3558-440A-894F-B085E93CA0C0}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2" xr:uid="{7CACC57F-85BA-475C-B464-4A0D739F2446}">
+      <formula1>"Economy,Premium Economy,Business Class,First Class"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{7F00C3A9-7054-48CB-9415-D75558C387D2}">
+      <formula1>"Hotel,Apartment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{22E7D3BA-BC19-4BD2-A2F0-41A4E8B8D251}">
+      <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2" xr:uid="{C743B37F-8D9F-460F-A95B-C4D15F90FB8B}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{8298AFF7-12EB-4EC7-843D-57AF497C7605}">
+      <formula1>"Hotel,Hotel+Flight,Hotel+Car,Hotel+Flight+Car,Hotel+Car+Flight"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2" xr:uid="{681655C7-2680-4E81-88BC-7B1A6884BC46}">
+      <formula1>"MasterCard,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CN2" xr:uid="{691485A4-56F5-4E89-915E-878C0472ADA7}">
+      <formula1>"5123456789012346,4111111111111111"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2" xr:uid="{36774B0E-B1B3-4101-A09C-72DCBA62A4BA}">
+      <formula1>"Quote,BookAndQuote,Fulfilment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2 BI2 BF2:BG2 AS2 AX2 AQ2 AV2 CE2 BA2" xr:uid="{C1D18C36-407B-418D-8074-39DBE74055A5}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2 AR2" xr:uid="{09D8F903-4326-4F29-980F-A8852D9B6FE3}">
+      <formula1>"Individual,Dependent,Personal,Guest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2 C2" xr:uid="{4FAE67B7-FC80-403E-A06E-C0B71A22A67D}">
+      <formula1>"sbt,preprod117,Live"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2" xr:uid="{52A13DCC-9D4F-4F91-8D0E-3D346255CAFB}">
+      <formula1>"OneWay,RoundTrip,MultiCity"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2" xr:uid="{F03DB7A9-F1C7-4CF2-B850-50D74B120857}">
+      <formula1>"Credit Card,Bill To Company"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{7C8D0438-2D94-44F0-8750-6E299B2297A9}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2" xr:uid="{B76F2910-F3EA-4F3E-AE90-37ADCE769FCA}">
+      <formula1>"SendForApproval,ProceedToCheckout"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{26B5F7EB-A061-4647-A78D-1493A6ECEA77}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{DE30A1E2-6D30-44AC-B747-805B8B961193}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{E753A255-06FE-478A-A4B8-B9F1FBB1A084}">
+      <formula1>"Old Url,SSO Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2 AA2" xr:uid="{17E02A78-25FC-4716-A198-B0FB115155FF}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="W2" r:id="rId1" display="Admin@123" xr:uid="{1380C751-8D95-4FC7-9E50-2F1EBF8C1E83}"/>
+    <hyperlink ref="F2" r:id="rId2" display="shubham.natkar@quadlabs.com" xr:uid="{A547C1E2-F688-4E99-BE9B-0DC0C25979AE}"/>
+    <hyperlink ref="G2" r:id="rId3" display="Password@123" xr:uid="{4DAE5536-55BF-4C10-BAF7-E9F97CC240DE}"/>
+    <hyperlink ref="R2" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{CE6A3C68-085A-401F-AB1A-085A4A3E577B}"/>
+    <hyperlink ref="AA2" r:id="rId5" display="shekhar.singh@quadlabs.com" xr:uid="{A3AF1591-4DFF-4135-BFFE-DB71F694A3F6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0213149D-792B-4B2B-A8E5-D4130C17BFBD}">
+  <dimension ref="A1:CQ5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD1" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF1" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG1" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="AM1" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN1" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AO1" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AP1" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="AQ1" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="AR1" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT1" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="AU1" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="AV1" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="AX1" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="AY1" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="BG1" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH1" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="BI1" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="BO1" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="BP1" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="BQ1" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="BX1" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="BY1" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="CA1" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="CB1" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="CC1" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="CD1" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="CE1" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="CF1" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="CG1" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="CH1" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="CI1" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="CJ1" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="CK1" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="CL1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="CM1" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="CN1" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="CO1" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="CP1" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="CQ1" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="R2" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA2" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD2" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE2" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF2" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG2" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="AH2" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="AI2" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM2" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AP2" s="24">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT2" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AU2" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW2" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB2" s="24">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE2" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG2" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BH2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ2" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="BK2" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM2" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN2" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP2" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR2" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="BS2" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="BT2" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="BU2" s="24">
+        <v>2</v>
+      </c>
+      <c r="BV2" s="24">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="24">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ2" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="CA2" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="CB2" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="CC2" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="CD2" s="24">
+        <v>25</v>
+      </c>
+      <c r="CE2" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG2" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH2" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="CI2" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ2" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CK2" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="CL2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM2" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="CN2" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO2" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP2" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="CQ2" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="R3" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="U3" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="V3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="W3" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="X3" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y3" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z3" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA3" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG3" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="AH3" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI3" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK3" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM3" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN3" s="24">
+        <v>3</v>
+      </c>
+      <c r="AO3" s="24">
+        <v>3</v>
+      </c>
+      <c r="AP3" s="24">
+        <v>3</v>
+      </c>
+      <c r="AQ3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT3" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AU3" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW3" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY3" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ3" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB3" s="24">
+        <v>2</v>
+      </c>
+      <c r="BC3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD3" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE3" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG3" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BH3" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ3" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="BK3" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM3" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN3" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="BO3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP3" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="BQ3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR3" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="BS3" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="BT3" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="BU3" s="24">
+        <v>2</v>
+      </c>
+      <c r="BV3" s="24">
+        <v>1</v>
+      </c>
+      <c r="BW3" s="24">
+        <v>1</v>
+      </c>
+      <c r="BX3" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ3" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="CA3" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="CB3" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="CC3" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="CD3" s="24">
+        <v>25</v>
+      </c>
+      <c r="CE3" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG3" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH3" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="CI3" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ3" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CK3" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="CL3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM3" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="CN3" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO3" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP3" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="CQ3" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="R4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="V4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="X4" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y4" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z4" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD4" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="AE4" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="AF4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG4" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="AH4" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="AI4" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL4" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM4" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN4" s="24">
+        <v>3</v>
+      </c>
+      <c r="AO4" s="24">
+        <v>3</v>
+      </c>
+      <c r="AP4" s="24">
+        <v>3</v>
+      </c>
+      <c r="AQ4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT4" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AU4" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW4" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY4" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ4" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB4" s="24">
+        <v>2</v>
+      </c>
+      <c r="BC4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE4" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG4" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BH4" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ4" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="BK4" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM4" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN4" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP4" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="BQ4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR4" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="BS4" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="BT4" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="BU4" s="24">
+        <v>2</v>
+      </c>
+      <c r="BV4" s="24">
+        <v>1</v>
+      </c>
+      <c r="BW4" s="24">
+        <v>1</v>
+      </c>
+      <c r="BX4" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ4" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="CA4" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="CB4" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="CC4" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="CD4" s="24">
+        <v>25</v>
+      </c>
+      <c r="CE4" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG4" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH4" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="CI4" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ4" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CK4" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="CL4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM4" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="CN4" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO4" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP4" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="CQ4" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="R5" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="U5" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="V5" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="X5" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y5" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z5" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA5" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD5" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE5" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="AF5" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG5" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="AH5" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="AI5" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK5" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL5" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM5" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN5" s="24">
+        <v>3</v>
+      </c>
+      <c r="AO5" s="24">
+        <v>3</v>
+      </c>
+      <c r="AP5" s="24">
+        <v>3</v>
+      </c>
+      <c r="AQ5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT5" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="AU5" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW5" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY5" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ5" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BB5" s="24">
+        <v>2</v>
+      </c>
+      <c r="BC5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD5" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE5" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG5" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BH5" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BJ5" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="BK5" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>238</v>
+      </c>
+      <c r="BM5" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN5" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="BO5" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP5" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="BQ5" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR5" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="BS5" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="BT5" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="BU5" s="24">
+        <v>2</v>
+      </c>
+      <c r="BV5" s="24">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="24">
+        <v>1</v>
+      </c>
+      <c r="BX5" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ5" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="CA5" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="CB5" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="CC5" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="CD5" s="24">
+        <v>25</v>
+      </c>
+      <c r="CE5" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF5" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG5" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH5" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="CI5" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ5" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="CK5" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="CL5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM5" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="CN5" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO5" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP5" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="CQ5" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5 AA2:AA5" xr:uid="{7114778B-8D97-4CF2-9F23-D4F00655B66A}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q5" xr:uid="{A1DA13B9-39F8-41E2-BFDC-A56F659BCEA4}">
+      <formula1>"Old Url,SSO Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W5" xr:uid="{583C1598-57B7-41A4-B56D-AB8C54612758}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T5" xr:uid="{8D3426FF-9F7A-46D1-B3FE-7B15DF398AC6}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CH5" xr:uid="{A688A683-8807-4229-A698-5B2B6265EDCF}">
+      <formula1>"SendForApproval,ProceedToCheckout"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC5" xr:uid="{AFE922ED-3D44-4B37-8944-38E833470EBA}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2:CL5" xr:uid="{EB179777-7A2F-440A-80AD-816A6FB54951}">
+      <formula1>"Credit Card,Bill To Company"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2:BN5" xr:uid="{BBF455DD-1623-4459-91AB-10841FE78C43}">
+      <formula1>"OneWay,RoundTrip,MultiCity"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O5 C2:C5" xr:uid="{CCC5D78C-9328-4883-A01D-C3C48CE6EE00}">
+      <formula1>"sbt,preprod117,Live"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB5 AR2:AR5" xr:uid="{9C75052D-23C8-47E2-B5D6-8C62200667EF}">
+      <formula1>"Individual,Dependent,Personal,Guest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2:BY5 BI2:BI5 BF2:BG5 AS2:AS5 AX2:AX5 AQ2:AQ5 AV2:AV5 CE2:CE5 BA2:BA5" xr:uid="{A974D21B-14FD-4383-89BC-D035617E034B}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK5" xr:uid="{DF171E48-B296-42E9-8C76-C478CA96113A}">
+      <formula1>"Quote,BookAndQuote,Fulfilment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CN2:CN5" xr:uid="{468305B0-EC7F-441D-B61A-124650CDED2F}">
+      <formula1>"5123456789012346,4111111111111111"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2:CM5" xr:uid="{6422A580-2AAF-43E1-A8A3-5926DB56584D}">
+      <formula1>"MasterCard,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM5" xr:uid="{402F6508-7028-45D1-8BA3-8BDC9E3F7D71}">
+      <formula1>"Hotel,Hotel+Flight,Hotel+Car,Hotel+Flight+Car,Hotel+Car+Flight"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI5" xr:uid="{9D306471-4246-4384-8052-956E25B9910C}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH5" xr:uid="{12E5D7CE-48D8-460D-9630-8566D0C153A3}">
+      <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2:BJ5" xr:uid="{A182058D-5F1D-4EAA-86E1-F51A16A173F6}">
+      <formula1>"Hotel,Apartment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2:BX5" xr:uid="{886427F1-DC66-467B-BE88-62484FEF3042}">
+      <formula1>"Economy,Premium Economy,Business Class,First Class"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2:BW5" xr:uid="{E7006B4B-BDF4-4B67-869E-9DCE4F64F7B0}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U5" xr:uid="{047D376B-B673-4442-BF51-1B7E5132E4A5}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V5" xr:uid="{F4339688-CBDD-4A27-A223-7C3DFD3BDCED}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y5" xr:uid="{DC7490D5-F6D3-4F1B-8576-F04E96012A1B}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X5" xr:uid="{8A8B0358-FED9-490E-AF9C-42C9D4B275DD}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z5" xr:uid="{4A3091D7-7A5A-4A7B-8BBD-2D5356733255}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CQ2:CQ5" xr:uid="{342A7FF7-1795-451F-A8E9-38C140876DE8}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar,Shekhar Singh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM5" xr:uid="{A9BEBBC4-6699-4C8C-A6E3-DC3224C1A190}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AF5 AW2:AW5" xr:uid="{31F15F7B-01E9-4E69-BF82-00148B03A7B7}">
+      <formula1>"5 KM,10 KM,20 KM,30 KM,40 KM,50 KM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5" xr:uid="{43C8C947-2AD6-43F5-A0A8-B4093B6C10E2}">
+      <formula1>"Laxmi@123,Password@123,Quad@720,Quad@721,Password@1234,Admin@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{30BD28B7-F552-460C-A3E7-16B81DEC1A92}">
+      <formula1>"Saurav_at,tarun"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{D332F7AD-0936-41C3-AE75-97D2391E34D4}">
+      <formula1>"at,QL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{CA39A78D-F873-4C0C-A254-747B57F3C7EC}">
+      <formula1>"//staging117/backoffice/,//preprod.quadlabs.net/backoffice/,//test.quadlabs.net/backoffice/"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{16D9E4C5-DF3E-47BA-ACD9-C86DE36FDF94}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5" xr:uid="{D0B6A6C4-7935-43FD-A044-AC254E518D46}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{09192170-88B7-451A-A0D5-FD804C1A0770}">
+      <formula1>"LUXURY COLLECTION,COURTYARD BY MARRIOTT"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="W2" r:id="rId1" display="Admin@123" xr:uid="{8E39D271-6A4C-476A-9811-EAB6B649B593}"/>
+    <hyperlink ref="F2" r:id="rId2" display="shubham.natkar@quadlabs.com" xr:uid="{31B9B08D-4364-4C52-88C6-2ECD248F07BC}"/>
+    <hyperlink ref="G2" r:id="rId3" display="Password@123" xr:uid="{5224655F-F48D-4CC6-A2A6-4A5409CF8889}"/>
+    <hyperlink ref="R2" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{4EFB36F1-FF29-4053-865E-F75FAC0BD11B}"/>
+    <hyperlink ref="AA2" r:id="rId5" display="shekhar.singh@quadlabs.com" xr:uid="{72985DB2-7B1D-4C92-BCEF-BAA1033D636A}"/>
+    <hyperlink ref="W3" r:id="rId6" display="Admin@123" xr:uid="{D75FFC89-EFB6-45A4-9C53-7090C07988D2}"/>
+    <hyperlink ref="F3" r:id="rId7" display="shubham.natkar@quadlabs.com" xr:uid="{BD512CC6-283D-494F-A40B-A4C8D2F377FC}"/>
+    <hyperlink ref="G3" r:id="rId8" display="Password@123" xr:uid="{8A4B7439-8A15-42DC-8C35-7E774EE94553}"/>
+    <hyperlink ref="R3" r:id="rId9" display="shekhar.singh@quadlabs.com" xr:uid="{D67915AD-46EE-4939-80AB-068E3E39666F}"/>
+    <hyperlink ref="AA3" r:id="rId10" display="shekhar.singh@quadlabs.com" xr:uid="{B41BC271-9738-4E5C-9608-100E0E123800}"/>
+    <hyperlink ref="W4" r:id="rId11" display="Admin@123" xr:uid="{E5366FA1-E907-49F5-994F-1061E7CAF916}"/>
+    <hyperlink ref="F4" r:id="rId12" display="shubham.natkar@quadlabs.com" xr:uid="{5CBFBB3C-427A-48F8-8707-F1F9CFE82CFC}"/>
+    <hyperlink ref="G4" r:id="rId13" display="Password@123" xr:uid="{C8AAF5CF-EB8F-404F-A1F2-F1B352F71B45}"/>
+    <hyperlink ref="R4" r:id="rId14" display="shekhar.singh@quadlabs.com" xr:uid="{41BCDAC6-5574-4C26-A4E0-79AFB1BF3FF2}"/>
+    <hyperlink ref="AA4" r:id="rId15" display="shekhar.singh@quadlabs.com" xr:uid="{9A6F45F4-FAC2-42E8-A9E4-E1893253774A}"/>
+    <hyperlink ref="W5" r:id="rId16" display="Admin@123" xr:uid="{87F48F79-985A-4D89-98F6-8C8B2178374E}"/>
+    <hyperlink ref="F5" r:id="rId17" display="shubham.natkar@quadlabs.com" xr:uid="{9DA2A3AE-23E1-4A8B-85EF-64D2CE5B6E0D}"/>
+    <hyperlink ref="G5" r:id="rId18" display="Password@123" xr:uid="{B84BDFD0-E2ED-4455-8541-F04C78296BEA}"/>
+    <hyperlink ref="R5" r:id="rId19" display="shekhar.singh@quadlabs.com" xr:uid="{42E6E6A5-5710-4E8B-BB03-945FF2B248B5}"/>
+    <hyperlink ref="AA5" r:id="rId20" display="shekhar.singh@quadlabs.com" xr:uid="{4D750C6B-FEC7-4CD7-8103-7DFDD4C5BBDB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04B49D8-9A43-44BD-8F63-39EEB9BA1789}">
   <dimension ref="A1:CQ2"/>
   <sheetViews>
@@ -4423,7 +6903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C3C0B8-E706-4C31-B9AD-3EE948CD9917}">
   <dimension ref="A1:CA2"/>
   <sheetViews>
@@ -5086,7 +7566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
@@ -5544,7 +8024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -5810,7 +8290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -6076,7 +8556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
@@ -6581,763 +9061,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AH4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH1" s="25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="P2" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="2">
-        <v>3</v>
-      </c>
-      <c r="W2" s="2">
-        <v>3</v>
-      </c>
-      <c r="X2" s="2">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>345678</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>123</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="P3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V3" s="2">
-        <v>3</v>
-      </c>
-      <c r="W3" s="2">
-        <v>3</v>
-      </c>
-      <c r="X3" s="2">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>345678</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>123</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH3" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="P4" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="2">
-        <v>0</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V4" s="2">
-        <v>3</v>
-      </c>
-      <c r="W4" s="2">
-        <v>3</v>
-      </c>
-      <c r="X4" s="2">
-        <v>3</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>345678</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>123</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH4" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-0600-000000000000}">
-      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0600-000001000000}">
-      <formula1>"Password@12345,GXPC6NWQVFKVOZG,Laxmi@123"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{00000000-0002-0000-0600-000002000000}">
-      <formula1>"Shubham1,Shubham,rsudesh15"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{00000000-0002-0000-0600-000003000000}">
-      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0600-000004000000}">
-      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{00000000-0002-0000-0600-000005000000}">
-      <formula1>"Prince Chaurasia,Gunjan Swain,Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{00000000-0002-0000-0600-000006000000}">
-      <formula1>"TravelArranger,Admin"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{00000000-0002-0000-0600-000007000000}">
-      <formula1>"sbt,preprod117"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="Password@12345" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="J2" r:id="rId2" display="prince.chaurasia@quadlabs.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="J3:J4" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="I3:I4" r:id="rId4" display="Password@12345" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AQ2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="O2" s="3">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>345678</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>123</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE4"/>
@@ -7802,6 +9525,763 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AH4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="P2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="2">
+        <v>3</v>
+      </c>
+      <c r="W2" s="2">
+        <v>3</v>
+      </c>
+      <c r="X2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>345678</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>123</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="2">
+        <v>3</v>
+      </c>
+      <c r="W3" s="2">
+        <v>3</v>
+      </c>
+      <c r="X3" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>345678</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>123</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH3" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="P4" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="2">
+        <v>3</v>
+      </c>
+      <c r="W4" s="2">
+        <v>3</v>
+      </c>
+      <c r="X4" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>345678</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>123</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH4" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-0600-000000000000}">
+      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0600-000001000000}">
+      <formula1>"Password@12345,GXPC6NWQVFKVOZG,Laxmi@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{00000000-0002-0000-0600-000002000000}">
+      <formula1>"Shubham1,Shubham,rsudesh15"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{00000000-0002-0000-0600-000003000000}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0600-000004000000}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{00000000-0002-0000-0600-000005000000}">
+      <formula1>"Prince Chaurasia,Gunjan Swain,Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{00000000-0002-0000-0600-000006000000}">
+      <formula1>"TravelArranger,Admin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{00000000-0002-0000-0600-000007000000}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="Password@12345" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" display="prince.chaurasia@quadlabs.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="J3:J4" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="I3:I4" r:id="rId4" display="Password@12345" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AQ2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="3">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>345678</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>123</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AU2"/>
   <sheetViews>
@@ -8115,7 +10595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
@@ -8496,7 +10976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -8679,7 +11159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -8838,7 +11318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -12784,7 +15264,7 @@
   <dimension ref="A1:CA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>